<commit_message>
"added enchanced PDE corrections to main"
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kiriakos/Documents/vs_code/DL_Democritos_ptyx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05FDC222-D14A-A44F-8E24-515AC9282A43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A33FE2B5-A754-0F43-B45E-03433AC64ACB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6520" yWindow="1580" windowWidth="28040" windowHeight="17440" xr2:uid="{D4F9D12D-A62D-DB48-ACCA-F2BA13E6C26D}"/>
+    <workbookView xWindow="14640" yWindow="3880" windowWidth="28040" windowHeight="17440" xr2:uid="{D4F9D12D-A62D-DB48-ACCA-F2BA13E6C26D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,15 +36,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="9">
   <si>
     <t>Data persentage</t>
   </si>
   <si>
     <t>RMSE</t>
-  </si>
-  <si>
-    <t>Ship</t>
   </si>
   <si>
     <t>Aframax</t>
@@ -63,6 +60,9 @@
   </si>
   <si>
     <t>Percentage Improvement</t>
+  </si>
+  <si>
+    <t>Danae</t>
   </si>
 </sst>
 </file>
@@ -116,7 +116,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -129,6 +129,9 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -463,10 +466,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80631562-7B5B-0A42-B36A-F3660D51C0D2}">
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0.2"/>
@@ -474,48 +477,49 @@
     <col min="1" max="1" width="10.83203125" style="1"/>
     <col min="2" max="2" width="19" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19" style="1" customWidth="1"/>
-    <col min="4" max="5" width="10.83203125" style="1"/>
-    <col min="6" max="6" width="28.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.83203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5" style="1" customWidth="1"/>
+    <col min="6" max="6" width="14.83203125" customWidth="1"/>
+    <col min="7" max="7" width="12.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="6"/>
+      <c r="F1" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="6"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="2">
-        <v>0</v>
-      </c>
-      <c r="B2" s="2">
-        <v>100</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="2">
-        <v>1784</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>0</v>
       </c>
@@ -523,36 +527,38 @@
         <v>100</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="4">
-        <v>1547</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F3" s="2">
-        <v>13.3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+      <c r="D3" s="2">
+        <v>1784</v>
+      </c>
+      <c r="E3" s="2">
+        <v>2735</v>
+      </c>
+      <c r="G3" s="1"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>0</v>
       </c>
       <c r="B4" s="2">
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="2">
-        <v>2001</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+        <v>6</v>
+      </c>
+      <c r="D4" s="4">
+        <v>1547</v>
+      </c>
+      <c r="E4" s="4">
+        <v>2685</v>
+      </c>
+      <c r="F4" s="2">
+        <v>13.3</v>
+      </c>
+      <c r="G4" s="1"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>0</v>
       </c>
@@ -560,36 +566,34 @@
         <v>20</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" s="4">
-        <v>1880</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F5" s="2">
-        <v>6.1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="3">
-        <v>3</v>
-      </c>
-      <c r="B6" s="3">
-        <v>100</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" s="3">
-        <v>1797</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+      <c r="D5" s="2">
+        <v>2001</v>
+      </c>
+      <c r="E5" s="2"/>
+      <c r="G5" s="1"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="2">
+        <v>0</v>
+      </c>
+      <c r="B6" s="2">
+        <v>20</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="4">
+        <v>1599</v>
+      </c>
+      <c r="E6" s="4"/>
+      <c r="F6" s="2">
+        <v>20.100000000000001</v>
+      </c>
+      <c r="G6" s="1"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="3">
         <v>3</v>
       </c>
@@ -597,36 +601,34 @@
         <v>100</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7" s="5">
-        <v>1184</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F7" s="3">
-        <v>34.200000000000003</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+      <c r="D7" s="3">
+        <v>1797</v>
+      </c>
+      <c r="E7" s="3"/>
+      <c r="G7" s="1"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="3">
         <v>3</v>
       </c>
       <c r="B8" s="3">
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8" s="3">
-        <v>2675</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+        <v>6</v>
+      </c>
+      <c r="D8" s="5">
+        <v>1184</v>
+      </c>
+      <c r="E8" s="5"/>
+      <c r="F8" s="3">
+        <v>34.200000000000003</v>
+      </c>
+      <c r="G8" s="1"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="3">
         <v>3</v>
       </c>
@@ -634,36 +636,34 @@
         <v>20</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D9" s="4">
+        <v>4</v>
+      </c>
+      <c r="D9" s="3">
+        <v>2675</v>
+      </c>
+      <c r="E9" s="3"/>
+      <c r="G9" s="1"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" s="3">
+        <v>3</v>
+      </c>
+      <c r="B10" s="3">
+        <v>20</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="4">
         <v>2101</v>
       </c>
-      <c r="E9" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F9" s="3">
+      <c r="E10" s="4"/>
+      <c r="F10" s="3">
         <v>21.5</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="3">
-        <v>5</v>
-      </c>
-      <c r="B10" s="3">
-        <v>100</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D10" s="3">
-        <v>1876</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G10" s="1"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="3">
         <v>5</v>
       </c>
@@ -671,36 +671,34 @@
         <v>100</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D11" s="4">
-        <v>1503</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F11" s="3">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+      <c r="D11" s="3">
+        <v>1876</v>
+      </c>
+      <c r="E11" s="3"/>
+      <c r="G11" s="1"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="3">
         <v>5</v>
       </c>
       <c r="B12" s="3">
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D12" s="3">
-        <v>2441</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+        <v>6</v>
+      </c>
+      <c r="D12" s="4">
+        <v>1503</v>
+      </c>
+      <c r="E12" s="4"/>
+      <c r="F12" s="3">
+        <v>20</v>
+      </c>
+      <c r="G12" s="1"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="3">
         <v>5</v>
       </c>
@@ -708,36 +706,34 @@
         <v>20</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D13" s="4">
+        <v>4</v>
+      </c>
+      <c r="D13" s="3">
+        <v>2441</v>
+      </c>
+      <c r="E13" s="3"/>
+      <c r="G13" s="1"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" s="3">
+        <v>5</v>
+      </c>
+      <c r="B14" s="3">
+        <v>20</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" s="4">
         <v>1868</v>
       </c>
-      <c r="E13" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F13" s="3">
+      <c r="E14" s="4"/>
+      <c r="F14" s="3">
         <v>23.5</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" s="3">
-        <v>7</v>
-      </c>
-      <c r="B14" s="3">
-        <v>100</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D14" s="3">
-        <v>3753</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G14" s="1"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="3">
         <v>7</v>
       </c>
@@ -745,36 +741,34 @@
         <v>100</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D15" s="4">
-        <v>1739</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F15" s="3">
-        <v>63.7</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+      <c r="D15" s="3">
+        <v>3753</v>
+      </c>
+      <c r="E15" s="3"/>
+      <c r="G15" s="1"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="3">
         <v>7</v>
       </c>
       <c r="B16" s="3">
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D16" s="3">
-        <v>3191</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+        <v>6</v>
+      </c>
+      <c r="D16" s="4">
+        <v>1739</v>
+      </c>
+      <c r="E16" s="4"/>
+      <c r="F16" s="3">
+        <v>63.7</v>
+      </c>
+      <c r="G16" s="1"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="3">
         <v>7</v>
       </c>
@@ -782,36 +776,34 @@
         <v>20</v>
       </c>
       <c r="C17" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D17" s="3">
+        <v>3191</v>
+      </c>
+      <c r="E17" s="3"/>
+      <c r="G17" s="1"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" s="3">
         <v>7</v>
       </c>
-      <c r="D17" s="4">
+      <c r="B18" s="3">
+        <v>20</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D18" s="4">
         <v>1389</v>
       </c>
-      <c r="E17" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F17" s="3">
+      <c r="E18" s="4"/>
+      <c r="F18" s="3">
         <v>56.5</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" s="2">
-        <v>9</v>
-      </c>
-      <c r="B18" s="2">
-        <v>100</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D18" s="2">
-        <v>2652</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G18" s="1"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
         <v>9</v>
       </c>
@@ -819,36 +811,40 @@
         <v>100</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D19" s="4">
-        <v>857</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F19" s="2">
-        <v>67.7</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+      <c r="D19" s="2">
+        <v>2652</v>
+      </c>
+      <c r="E19" s="2">
+        <v>1510</v>
+      </c>
+      <c r="G19" s="1"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <v>9</v>
       </c>
       <c r="B20" s="2">
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D20" s="2">
-        <v>3163</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+        <v>6</v>
+      </c>
+      <c r="D20" s="4">
+        <v>857</v>
+      </c>
+      <c r="E20" s="4">
+        <v>1053</v>
+      </c>
+      <c r="F20" s="2">
+        <v>67.7</v>
+      </c>
+      <c r="G20" s="2">
+        <v>30.3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
         <v>9</v>
       </c>
@@ -856,19 +852,38 @@
         <v>20</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D21" s="4">
+        <v>4</v>
+      </c>
+      <c r="D21" s="2">
+        <v>3163</v>
+      </c>
+      <c r="E21" s="2"/>
+      <c r="G21" s="1"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22" s="2">
+        <v>9</v>
+      </c>
+      <c r="B22" s="2">
+        <v>20</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D22" s="4">
         <v>1813</v>
       </c>
-      <c r="E21" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F21" s="2">
+      <c r="E22" s="4"/>
+      <c r="F22" s="2">
         <v>42.6</v>
       </c>
+      <c r="G22" s="1"/>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:G1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>